<commit_message>
Updated RQ1, RQ2 and Readme files
</commit_message>
<xml_diff>
--- a/experiments/RQ2.xlsx
+++ b/experiments/RQ2.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seungyeob.shin/Repository/models2018-mosis/artifact/experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karim.chaouch/HITECS/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BF2066FA-007C-CF4F-BBAB-6F7A4FE66640}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="5360" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="920" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
     <sheet name="Actual" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -413,20 +412,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3001"/>
   <sheetViews>
-    <sheetView topLeftCell="A2989" workbookViewId="0">
-      <selection activeCell="D3010" sqref="D3010"/>
+    <sheetView topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="4" customWidth="1"/>
     <col min="2" max="4" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -69459,11 +69459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>